<commit_message>
Finish money and life mechanism
变更概述：
新增扣血机制和金币系统（杀怪掉金币，造塔花金币，怪走到中间扣血）

其他修改：
更换了地板贴图，稍微没那么难看（但还是很难看-_-!!!）

Signed-off-by: Qi Lin <kylin9749@foxmail.com>
</commit_message>
<xml_diff>
--- a/游戏开发文档/程序需求表格.xlsx
+++ b/游戏开发文档/程序需求表格.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
   <si>
     <t xml:space="preserve">模块</t>
   </si>
@@ -180,6 +180,21 @@
   </si>
   <si>
     <t xml:space="preserve">主动释放技能的流程</t>
+  </si>
+  <si>
+    <t xml:space="preserve">关卡机制</t>
+  </si>
+  <si>
+    <t xml:space="preserve">机械时钟</t>
+  </si>
+  <si>
+    <t xml:space="preserve">机械时钟的指针会遮挡防御塔</t>
+  </si>
+  <si>
+    <t xml:space="preserve">电子表</t>
+  </si>
+  <si>
+    <t xml:space="preserve">电子表未出现的数字处的防御塔会消失</t>
   </si>
 </sst>
 </file>
@@ -280,7 +295,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -316,6 +331,13 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -342,68 +364,80 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -656,177 +690,177 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
+      <selection pane="topLeft" activeCell="D22" activeCellId="0" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.43359375" defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="55.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="23.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="18.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="21.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="55.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="10.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="23.42"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="3" t="n">
+      <c r="D2" s="4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2"/>
-      <c r="B3" s="4" t="s">
+      <c r="A3" s="3"/>
+      <c r="B3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="4" t="n">
+      <c r="D3" s="5" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2"/>
-      <c r="B4" s="5" t="s">
+      <c r="A4" s="3"/>
+      <c r="B4" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="E4" s="0" t="s">
+      <c r="D4" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2"/>
-      <c r="B5" s="3" t="s">
+      <c r="A5" s="3"/>
+      <c r="B5" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="3" t="n">
+      <c r="D5" s="4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="36.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2"/>
-      <c r="B6" s="3" t="s">
+      <c r="A6" s="3"/>
+      <c r="B6" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="3" t="n">
+      <c r="D6" s="4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2"/>
-      <c r="B7" s="4" t="s">
+      <c r="A7" s="3"/>
+      <c r="B7" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="4" t="n">
-        <v>0</v>
+      <c r="D7" s="5" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2"/>
-      <c r="B8" s="3" t="s">
+      <c r="A8" s="3"/>
+      <c r="B8" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="3" t="n">
+      <c r="D8" s="4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2"/>
-      <c r="B9" s="3" t="s">
+      <c r="A9" s="3"/>
+      <c r="B9" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="3" t="n">
+      <c r="D9" s="4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="2"/>
-      <c r="B10" s="5" t="s">
+      <c r="A10" s="3"/>
+      <c r="B10" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D10" s="5" t="n">
-        <v>0</v>
+      <c r="D10" s="6" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="2"/>
-      <c r="B11" s="3" t="s">
+      <c r="A11" s="3"/>
+      <c r="B11" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="3" t="n">
+      <c r="D11" s="4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="2"/>
-      <c r="B12" s="3" t="s">
+      <c r="A12" s="3"/>
+      <c r="B12" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D12" s="3" t="n">
+      <c r="D12" s="4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="2"/>
+      <c r="A13" s="3"/>
       <c r="B13" s="4" t="s">
         <v>29</v>
       </c>
@@ -838,118 +872,141 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D14" s="4" t="n">
-        <v>0</v>
+      <c r="D14" s="5" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="6"/>
-      <c r="B15" s="5" t="s">
+      <c r="A15" s="7"/>
+      <c r="B15" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C15" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="D15" s="5" t="n">
-        <v>0</v>
+      <c r="D15" s="6" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="6"/>
-      <c r="B16" s="4" t="s">
+      <c r="A16" s="7"/>
+      <c r="B16" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="D16" s="4" t="n">
-        <v>0</v>
+      <c r="D16" s="5" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="7" t="s">
+      <c r="A17" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="D17" s="5" t="n">
+      <c r="D17" s="6" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="7"/>
-      <c r="B18" s="3" t="s">
+      <c r="A18" s="8"/>
+      <c r="B18" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C18" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="D18" s="3" t="n">
+      <c r="D18" s="4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="7" t="s">
+      <c r="A19" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B19" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="C19" s="5" t="s">
+      <c r="C19" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="D19" s="5" t="n">
+      <c r="D19" s="6" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="7"/>
-      <c r="B20" s="4" t="s">
+      <c r="A20" s="8"/>
+      <c r="B20" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C20" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="D20" s="4" t="n">
+      <c r="D20" s="5" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="5" t="s">
+      <c r="A21" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B21" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="C21" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="D21" s="5" t="n">
+      <c r="D21" s="6" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="4" t="s">
+      <c r="A22" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4" t="s">
+      <c r="B22" s="5"/>
+      <c r="C22" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="D22" s="4"/>
+      <c r="D22" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="D23" s="9"/>
+    </row>
+    <row r="24" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B24" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="D24" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -976,417 +1033,417 @@
   <dimension ref="A1:AD13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AA17" activeCellId="0" sqref="AA17"/>
+      <selection pane="topLeft" activeCell="O9" activeCellId="0" sqref="O9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4.58984375" defaultRowHeight="21.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="4.578125" defaultRowHeight="21.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="1" style="8" width="4.58"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="1" style="10" width="4.58"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="9"/>
-      <c r="B1" s="10"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="11"/>
-      <c r="L1" s="10"/>
-      <c r="M1" s="11"/>
-      <c r="N1" s="10"/>
-      <c r="O1" s="11"/>
-      <c r="P1" s="10"/>
-      <c r="Q1" s="11"/>
-      <c r="R1" s="10"/>
-      <c r="S1" s="11"/>
-      <c r="T1" s="10"/>
-      <c r="U1" s="11"/>
-      <c r="V1" s="10"/>
-      <c r="W1" s="11"/>
-      <c r="X1" s="10"/>
-      <c r="Y1" s="11"/>
-      <c r="Z1" s="10"/>
-      <c r="AA1" s="11"/>
-      <c r="AB1" s="10"/>
-      <c r="AC1" s="9"/>
+      <c r="A1" s="11"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="13"/>
+      <c r="N1" s="12"/>
+      <c r="O1" s="13"/>
+      <c r="P1" s="12"/>
+      <c r="Q1" s="13"/>
+      <c r="R1" s="12"/>
+      <c r="S1" s="13"/>
+      <c r="T1" s="12"/>
+      <c r="U1" s="13"/>
+      <c r="V1" s="12"/>
+      <c r="W1" s="13"/>
+      <c r="X1" s="12"/>
+      <c r="Y1" s="13"/>
+      <c r="Z1" s="12"/>
+      <c r="AA1" s="13"/>
+      <c r="AB1" s="12"/>
+      <c r="AC1" s="11"/>
     </row>
     <row r="2" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="10"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
-      <c r="K2" s="10"/>
-      <c r="L2" s="10"/>
-      <c r="M2" s="10"/>
-      <c r="N2" s="10"/>
-      <c r="O2" s="10"/>
-      <c r="P2" s="10"/>
-      <c r="Q2" s="10"/>
-      <c r="R2" s="10"/>
-      <c r="S2" s="10"/>
-      <c r="T2" s="10"/>
-      <c r="U2" s="10"/>
-      <c r="V2" s="10"/>
-      <c r="W2" s="10"/>
-      <c r="X2" s="10"/>
-      <c r="Y2" s="10"/>
-      <c r="Z2" s="10"/>
-      <c r="AA2" s="10"/>
-      <c r="AB2" s="10"/>
-      <c r="AC2" s="10"/>
+      <c r="A2" s="12"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
+      <c r="K2" s="12"/>
+      <c r="L2" s="12"/>
+      <c r="M2" s="12"/>
+      <c r="N2" s="12"/>
+      <c r="O2" s="12"/>
+      <c r="P2" s="12"/>
+      <c r="Q2" s="12"/>
+      <c r="R2" s="12"/>
+      <c r="S2" s="12"/>
+      <c r="T2" s="12"/>
+      <c r="U2" s="12"/>
+      <c r="V2" s="12"/>
+      <c r="W2" s="12"/>
+      <c r="X2" s="12"/>
+      <c r="Y2" s="12"/>
+      <c r="Z2" s="12"/>
+      <c r="AA2" s="12"/>
+      <c r="AB2" s="12"/>
+      <c r="AC2" s="12"/>
     </row>
     <row r="3" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="9"/>
-      <c r="B3" s="10"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="12"/>
-      <c r="J3" s="13"/>
-      <c r="K3" s="12"/>
-      <c r="L3" s="13"/>
-      <c r="M3" s="12"/>
-      <c r="N3" s="10"/>
-      <c r="O3" s="14"/>
-      <c r="P3" s="10"/>
-      <c r="Q3" s="12"/>
-      <c r="R3" s="13"/>
-      <c r="S3" s="12"/>
-      <c r="T3" s="13"/>
-      <c r="U3" s="12"/>
-      <c r="V3" s="10"/>
-      <c r="W3" s="12"/>
-      <c r="X3" s="13"/>
-      <c r="Y3" s="12"/>
-      <c r="Z3" s="13"/>
-      <c r="AA3" s="12"/>
-      <c r="AB3" s="10"/>
-      <c r="AC3" s="9"/>
+      <c r="A3" s="11"/>
+      <c r="B3" s="12"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="15"/>
+      <c r="K3" s="14"/>
+      <c r="L3" s="15"/>
+      <c r="M3" s="14"/>
+      <c r="N3" s="12"/>
+      <c r="O3" s="16"/>
+      <c r="P3" s="12"/>
+      <c r="Q3" s="14"/>
+      <c r="R3" s="15"/>
+      <c r="S3" s="14"/>
+      <c r="T3" s="15"/>
+      <c r="U3" s="14"/>
+      <c r="V3" s="12"/>
+      <c r="W3" s="14"/>
+      <c r="X3" s="15"/>
+      <c r="Y3" s="14"/>
+      <c r="Z3" s="15"/>
+      <c r="AA3" s="14"/>
+      <c r="AB3" s="12"/>
+      <c r="AC3" s="11"/>
     </row>
     <row r="4" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="10"/>
-      <c r="B4" s="10"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="10"/>
-      <c r="L4" s="10"/>
-      <c r="M4" s="13"/>
-      <c r="N4" s="10"/>
-      <c r="O4" s="10"/>
-      <c r="P4" s="10"/>
-      <c r="Q4" s="13"/>
-      <c r="R4" s="10"/>
-      <c r="S4" s="10"/>
-      <c r="T4" s="10"/>
-      <c r="U4" s="13"/>
-      <c r="V4" s="10"/>
-      <c r="W4" s="13"/>
-      <c r="X4" s="10"/>
-      <c r="Y4" s="10"/>
-      <c r="Z4" s="10"/>
-      <c r="AA4" s="13"/>
-      <c r="AB4" s="10"/>
-      <c r="AC4" s="10"/>
+      <c r="A4" s="12"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="15"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="12"/>
+      <c r="L4" s="12"/>
+      <c r="M4" s="15"/>
+      <c r="N4" s="12"/>
+      <c r="O4" s="12"/>
+      <c r="P4" s="12"/>
+      <c r="Q4" s="15"/>
+      <c r="R4" s="12"/>
+      <c r="S4" s="12"/>
+      <c r="T4" s="12"/>
+      <c r="U4" s="15"/>
+      <c r="V4" s="12"/>
+      <c r="W4" s="15"/>
+      <c r="X4" s="12"/>
+      <c r="Y4" s="12"/>
+      <c r="Z4" s="12"/>
+      <c r="AA4" s="15"/>
+      <c r="AB4" s="12"/>
+      <c r="AC4" s="12"/>
     </row>
     <row r="5" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="9"/>
-      <c r="B5" s="10"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="10"/>
-      <c r="K5" s="14"/>
-      <c r="L5" s="10"/>
-      <c r="M5" s="12"/>
-      <c r="N5" s="10"/>
-      <c r="O5" s="12"/>
-      <c r="P5" s="10"/>
-      <c r="Q5" s="12"/>
-      <c r="R5" s="10"/>
-      <c r="S5" s="14"/>
-      <c r="T5" s="10"/>
-      <c r="U5" s="12"/>
-      <c r="V5" s="10"/>
-      <c r="W5" s="12"/>
-      <c r="X5" s="10"/>
-      <c r="Y5" s="14"/>
-      <c r="Z5" s="10"/>
-      <c r="AA5" s="12"/>
-      <c r="AB5" s="10"/>
-      <c r="AC5" s="9"/>
+      <c r="A5" s="11"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="16"/>
+      <c r="L5" s="12"/>
+      <c r="M5" s="14"/>
+      <c r="N5" s="12"/>
+      <c r="O5" s="14"/>
+      <c r="P5" s="12"/>
+      <c r="Q5" s="14"/>
+      <c r="R5" s="12"/>
+      <c r="S5" s="16"/>
+      <c r="T5" s="12"/>
+      <c r="U5" s="14"/>
+      <c r="V5" s="12"/>
+      <c r="W5" s="14"/>
+      <c r="X5" s="12"/>
+      <c r="Y5" s="16"/>
+      <c r="Z5" s="12"/>
+      <c r="AA5" s="14"/>
+      <c r="AB5" s="12"/>
+      <c r="AC5" s="11"/>
     </row>
     <row r="6" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="10"/>
-      <c r="B6" s="10"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="13"/>
-      <c r="J6" s="10"/>
-      <c r="K6" s="10"/>
-      <c r="L6" s="10"/>
-      <c r="M6" s="13"/>
-      <c r="N6" s="10"/>
-      <c r="O6" s="10"/>
-      <c r="P6" s="10"/>
-      <c r="Q6" s="13"/>
-      <c r="R6" s="10"/>
-      <c r="S6" s="10"/>
-      <c r="T6" s="10"/>
-      <c r="U6" s="13"/>
-      <c r="V6" s="10"/>
-      <c r="W6" s="13"/>
-      <c r="X6" s="10"/>
-      <c r="Y6" s="10"/>
-      <c r="Z6" s="10"/>
-      <c r="AA6" s="13"/>
-      <c r="AB6" s="10"/>
-      <c r="AC6" s="10"/>
+      <c r="A6" s="12"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="12"/>
+      <c r="K6" s="12"/>
+      <c r="L6" s="12"/>
+      <c r="M6" s="15"/>
+      <c r="N6" s="12"/>
+      <c r="O6" s="12"/>
+      <c r="P6" s="12"/>
+      <c r="Q6" s="15"/>
+      <c r="R6" s="12"/>
+      <c r="S6" s="12"/>
+      <c r="T6" s="12"/>
+      <c r="U6" s="15"/>
+      <c r="V6" s="12"/>
+      <c r="W6" s="15"/>
+      <c r="X6" s="12"/>
+      <c r="Y6" s="12"/>
+      <c r="Z6" s="12"/>
+      <c r="AA6" s="15"/>
+      <c r="AB6" s="12"/>
+      <c r="AC6" s="12"/>
     </row>
     <row r="7" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="9"/>
-      <c r="B7" s="10"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="12"/>
-      <c r="J7" s="13"/>
-      <c r="K7" s="12"/>
-      <c r="L7" s="13"/>
-      <c r="M7" s="12"/>
-      <c r="N7" s="10"/>
-      <c r="O7" s="15"/>
-      <c r="P7" s="10"/>
-      <c r="Q7" s="12"/>
-      <c r="R7" s="13"/>
-      <c r="S7" s="12"/>
-      <c r="T7" s="13"/>
-      <c r="U7" s="12"/>
-      <c r="V7" s="10"/>
-      <c r="W7" s="12"/>
-      <c r="X7" s="13"/>
-      <c r="Y7" s="12"/>
-      <c r="Z7" s="13"/>
-      <c r="AA7" s="12"/>
-      <c r="AB7" s="10"/>
-      <c r="AC7" s="9"/>
+      <c r="A7" s="11"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="15"/>
+      <c r="K7" s="14"/>
+      <c r="L7" s="15"/>
+      <c r="M7" s="14"/>
+      <c r="N7" s="12"/>
+      <c r="O7" s="17"/>
+      <c r="P7" s="12"/>
+      <c r="Q7" s="14"/>
+      <c r="R7" s="15"/>
+      <c r="S7" s="14"/>
+      <c r="T7" s="15"/>
+      <c r="U7" s="14"/>
+      <c r="V7" s="12"/>
+      <c r="W7" s="14"/>
+      <c r="X7" s="15"/>
+      <c r="Y7" s="14"/>
+      <c r="Z7" s="15"/>
+      <c r="AA7" s="14"/>
+      <c r="AB7" s="12"/>
+      <c r="AC7" s="11"/>
     </row>
     <row r="8" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="10"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="13"/>
-      <c r="J8" s="10"/>
-      <c r="K8" s="10"/>
-      <c r="L8" s="10"/>
-      <c r="M8" s="13"/>
-      <c r="N8" s="10"/>
-      <c r="O8" s="10"/>
-      <c r="P8" s="10"/>
-      <c r="Q8" s="13"/>
-      <c r="R8" s="10"/>
-      <c r="S8" s="10"/>
-      <c r="T8" s="10"/>
-      <c r="U8" s="13"/>
-      <c r="V8" s="10"/>
-      <c r="W8" s="13"/>
-      <c r="X8" s="10"/>
-      <c r="Y8" s="10"/>
-      <c r="Z8" s="10"/>
-      <c r="AA8" s="13"/>
-      <c r="AB8" s="10"/>
-      <c r="AC8" s="10"/>
+      <c r="A8" s="12"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="12"/>
+      <c r="K8" s="12"/>
+      <c r="L8" s="12"/>
+      <c r="M8" s="15"/>
+      <c r="N8" s="12"/>
+      <c r="O8" s="12"/>
+      <c r="P8" s="12"/>
+      <c r="Q8" s="15"/>
+      <c r="R8" s="12"/>
+      <c r="S8" s="12"/>
+      <c r="T8" s="12"/>
+      <c r="U8" s="15"/>
+      <c r="V8" s="12"/>
+      <c r="W8" s="15"/>
+      <c r="X8" s="12"/>
+      <c r="Y8" s="12"/>
+      <c r="Z8" s="12"/>
+      <c r="AA8" s="15"/>
+      <c r="AB8" s="12"/>
+      <c r="AC8" s="12"/>
     </row>
     <row r="9" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="9"/>
-      <c r="B9" s="10"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="12"/>
-      <c r="J9" s="10"/>
-      <c r="K9" s="14"/>
-      <c r="L9" s="10"/>
-      <c r="M9" s="12"/>
-      <c r="N9" s="10"/>
-      <c r="O9" s="12"/>
-      <c r="P9" s="10"/>
-      <c r="Q9" s="12"/>
-      <c r="R9" s="10"/>
-      <c r="S9" s="14"/>
-      <c r="T9" s="10"/>
-      <c r="U9" s="12"/>
-      <c r="V9" s="10"/>
-      <c r="W9" s="12"/>
-      <c r="X9" s="10"/>
-      <c r="Y9" s="14"/>
-      <c r="Z9" s="10"/>
-      <c r="AA9" s="12"/>
-      <c r="AB9" s="10"/>
-      <c r="AC9" s="9"/>
+      <c r="A9" s="11"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="12"/>
+      <c r="K9" s="16"/>
+      <c r="L9" s="12"/>
+      <c r="M9" s="14"/>
+      <c r="N9" s="12"/>
+      <c r="O9" s="14"/>
+      <c r="P9" s="12"/>
+      <c r="Q9" s="14"/>
+      <c r="R9" s="12"/>
+      <c r="S9" s="16"/>
+      <c r="T9" s="12"/>
+      <c r="U9" s="14"/>
+      <c r="V9" s="12"/>
+      <c r="W9" s="14"/>
+      <c r="X9" s="12"/>
+      <c r="Y9" s="16"/>
+      <c r="Z9" s="12"/>
+      <c r="AA9" s="14"/>
+      <c r="AB9" s="12"/>
+      <c r="AC9" s="11"/>
     </row>
     <row r="10" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="10"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="13"/>
-      <c r="J10" s="10"/>
-      <c r="K10" s="10"/>
-      <c r="L10" s="10"/>
-      <c r="M10" s="13"/>
-      <c r="N10" s="10"/>
-      <c r="O10" s="10"/>
-      <c r="P10" s="10"/>
-      <c r="Q10" s="13"/>
-      <c r="R10" s="10"/>
-      <c r="S10" s="10"/>
-      <c r="T10" s="10"/>
-      <c r="U10" s="13"/>
-      <c r="V10" s="10"/>
-      <c r="W10" s="13"/>
-      <c r="X10" s="10"/>
-      <c r="Y10" s="10"/>
-      <c r="Z10" s="10"/>
-      <c r="AA10" s="13"/>
-      <c r="AB10" s="10"/>
-      <c r="AC10" s="10"/>
+      <c r="A10" s="12"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="15"/>
+      <c r="J10" s="12"/>
+      <c r="K10" s="12"/>
+      <c r="L10" s="12"/>
+      <c r="M10" s="15"/>
+      <c r="N10" s="12"/>
+      <c r="O10" s="12"/>
+      <c r="P10" s="12"/>
+      <c r="Q10" s="15"/>
+      <c r="R10" s="12"/>
+      <c r="S10" s="12"/>
+      <c r="T10" s="12"/>
+      <c r="U10" s="15"/>
+      <c r="V10" s="12"/>
+      <c r="W10" s="15"/>
+      <c r="X10" s="12"/>
+      <c r="Y10" s="12"/>
+      <c r="Z10" s="12"/>
+      <c r="AA10" s="15"/>
+      <c r="AB10" s="12"/>
+      <c r="AC10" s="12"/>
     </row>
     <row r="11" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="9"/>
-      <c r="B11" s="10"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="10"/>
-      <c r="I11" s="12"/>
-      <c r="J11" s="13"/>
-      <c r="K11" s="12"/>
-      <c r="L11" s="13"/>
-      <c r="M11" s="12"/>
-      <c r="N11" s="10"/>
-      <c r="O11" s="14"/>
-      <c r="P11" s="10"/>
-      <c r="Q11" s="12"/>
-      <c r="R11" s="13"/>
-      <c r="S11" s="12"/>
-      <c r="T11" s="13"/>
-      <c r="U11" s="12"/>
-      <c r="V11" s="10"/>
-      <c r="W11" s="12"/>
-      <c r="X11" s="13"/>
-      <c r="Y11" s="12"/>
-      <c r="Z11" s="13"/>
-      <c r="AA11" s="12"/>
-      <c r="AB11" s="10"/>
-      <c r="AC11" s="9"/>
-      <c r="AD11" s="9"/>
+      <c r="A11" s="11"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="15"/>
+      <c r="K11" s="14"/>
+      <c r="L11" s="15"/>
+      <c r="M11" s="14"/>
+      <c r="N11" s="12"/>
+      <c r="O11" s="16"/>
+      <c r="P11" s="12"/>
+      <c r="Q11" s="14"/>
+      <c r="R11" s="15"/>
+      <c r="S11" s="14"/>
+      <c r="T11" s="15"/>
+      <c r="U11" s="14"/>
+      <c r="V11" s="12"/>
+      <c r="W11" s="14"/>
+      <c r="X11" s="15"/>
+      <c r="Y11" s="14"/>
+      <c r="Z11" s="15"/>
+      <c r="AA11" s="14"/>
+      <c r="AB11" s="12"/>
+      <c r="AC11" s="11"/>
+      <c r="AD11" s="18"/>
     </row>
     <row r="12" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="10"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="10"/>
-      <c r="J12" s="10"/>
-      <c r="K12" s="10"/>
-      <c r="L12" s="10"/>
-      <c r="M12" s="10"/>
-      <c r="N12" s="10"/>
-      <c r="O12" s="10"/>
-      <c r="P12" s="10"/>
-      <c r="Q12" s="10"/>
-      <c r="R12" s="10"/>
-      <c r="S12" s="10"/>
-      <c r="T12" s="10"/>
-      <c r="U12" s="10"/>
-      <c r="V12" s="10"/>
-      <c r="W12" s="10"/>
-      <c r="X12" s="10"/>
-      <c r="Y12" s="10"/>
-      <c r="Z12" s="10"/>
-      <c r="AA12" s="10"/>
-      <c r="AB12" s="10"/>
-      <c r="AC12" s="10"/>
+      <c r="A12" s="12"/>
+      <c r="B12" s="12"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="12"/>
+      <c r="J12" s="12"/>
+      <c r="K12" s="12"/>
+      <c r="L12" s="12"/>
+      <c r="M12" s="12"/>
+      <c r="N12" s="12"/>
+      <c r="O12" s="12"/>
+      <c r="P12" s="12"/>
+      <c r="Q12" s="12"/>
+      <c r="R12" s="12"/>
+      <c r="S12" s="12"/>
+      <c r="T12" s="12"/>
+      <c r="U12" s="12"/>
+      <c r="V12" s="12"/>
+      <c r="W12" s="12"/>
+      <c r="X12" s="12"/>
+      <c r="Y12" s="12"/>
+      <c r="Z12" s="12"/>
+      <c r="AA12" s="12"/>
+      <c r="AB12" s="12"/>
+      <c r="AC12" s="12"/>
     </row>
     <row r="13" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="9"/>
-      <c r="B13" s="10"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="11"/>
-      <c r="J13" s="10"/>
-      <c r="K13" s="11"/>
-      <c r="L13" s="10"/>
-      <c r="M13" s="11"/>
-      <c r="N13" s="10"/>
-      <c r="O13" s="11"/>
-      <c r="P13" s="10"/>
-      <c r="Q13" s="11"/>
-      <c r="R13" s="10"/>
-      <c r="S13" s="11"/>
-      <c r="T13" s="10"/>
-      <c r="U13" s="11"/>
-      <c r="V13" s="10"/>
-      <c r="W13" s="11"/>
-      <c r="X13" s="10"/>
-      <c r="Y13" s="11"/>
-      <c r="Z13" s="10"/>
-      <c r="AA13" s="11"/>
-      <c r="AB13" s="10"/>
-      <c r="AC13" s="9"/>
+      <c r="A13" s="11"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="13"/>
+      <c r="J13" s="12"/>
+      <c r="K13" s="13"/>
+      <c r="L13" s="12"/>
+      <c r="M13" s="13"/>
+      <c r="N13" s="12"/>
+      <c r="O13" s="13"/>
+      <c r="P13" s="12"/>
+      <c r="Q13" s="13"/>
+      <c r="R13" s="12"/>
+      <c r="S13" s="13"/>
+      <c r="T13" s="12"/>
+      <c r="U13" s="13"/>
+      <c r="V13" s="12"/>
+      <c r="W13" s="13"/>
+      <c r="X13" s="12"/>
+      <c r="Y13" s="13"/>
+      <c r="Z13" s="12"/>
+      <c r="AA13" s="13"/>
+      <c r="AB13" s="12"/>
+      <c r="AC13" s="11"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>